<commit_message>
Update thuat toán xếp container.xlsx
</commit_message>
<xml_diff>
--- a/sort_container/thuat toán xếp container.xlsx
+++ b/sort_container/thuat toán xếp container.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t>w</t>
   </si>
@@ -148,6 +148,66 @@
   </si>
   <si>
     <t>o(n^2/4)</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>2(1,2)</t>
+  </si>
+  <si>
+    <t>1(3,4)</t>
+  </si>
+  <si>
+    <t>9(1)</t>
+  </si>
+  <si>
+    <t>7(2)</t>
+  </si>
+  <si>
+    <t>6(3)</t>
+  </si>
+  <si>
+    <t>5(4)</t>
+  </si>
+  <si>
+    <t>2(5)</t>
+  </si>
+  <si>
+    <t>1(6)</t>
+  </si>
+  <si>
+    <t>1(5,6)</t>
+  </si>
+  <si>
+    <t>1((1,2),(3,4))</t>
+  </si>
+  <si>
+    <t>(1,2)</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>5,6</t>
+  </si>
+  <si>
+    <t>1(1,2)(5,6)</t>
+  </si>
+  <si>
+    <t>t= 15</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>n =6</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -177,7 +237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,8 +272,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -249,13 +315,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -285,6 +360,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -567,236 +645,249 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:O64"/>
+  <dimension ref="A1:Q109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="D41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D1" s="9">
+        <v>95</v>
+      </c>
+      <c r="E1" s="9">
+        <v>89</v>
+      </c>
+      <c r="F1" s="9">
+        <v>79</v>
+      </c>
+      <c r="G1" s="9">
+        <v>75</v>
+      </c>
+      <c r="H1" s="9">
+        <v>73</v>
+      </c>
+      <c r="I1" s="9">
+        <f>SUM(D1:H1)</f>
+        <v>411</v>
+      </c>
+    </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <v>7</v>
-      </c>
-      <c r="K3">
-        <v>8</v>
-      </c>
-      <c r="L3">
-        <v>9</v>
-      </c>
-      <c r="M3">
-        <v>10</v>
+      <c r="D3" s="9">
+        <v>90</v>
+      </c>
+      <c r="E3" s="9">
+        <v>90</v>
+      </c>
+      <c r="F3" s="9">
+        <v>84</v>
+      </c>
+      <c r="G3" s="9">
+        <v>74</v>
+      </c>
+      <c r="H3" s="13">
+        <v>70</v>
+      </c>
+      <c r="I3" s="9">
+        <f>SUM(D3:H3)</f>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>9</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>95</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>90</v>
       </c>
-      <c r="F4">
+      <c r="F5">
+        <v>89</v>
+      </c>
+      <c r="G5">
         <v>90</v>
       </c>
-      <c r="G4">
-        <v>89</v>
-      </c>
-      <c r="H4">
+      <c r="H5">
         <v>79</v>
       </c>
-      <c r="I4">
+      <c r="I5">
         <v>84</v>
       </c>
-      <c r="J4">
+      <c r="J5">
         <v>75</v>
       </c>
-      <c r="K4">
+      <c r="K5">
         <v>74</v>
       </c>
-      <c r="L4">
+      <c r="L5">
+        <v>73</v>
+      </c>
+      <c r="M5">
         <v>70</v>
-      </c>
-      <c r="M4">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C5" s="2">
-        <f>L3</f>
-        <v>9</v>
-      </c>
-      <c r="D5" s="2">
-        <f>J3</f>
-        <v>7</v>
-      </c>
-      <c r="E5" s="2">
-        <f>H3</f>
-        <v>5</v>
-      </c>
-      <c r="F5" s="2">
-        <f>F3</f>
-        <v>3</v>
-      </c>
-      <c r="G5" s="2">
-        <f>D3</f>
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
-        <f>E3</f>
-        <v>2</v>
-      </c>
-      <c r="I5" s="1">
-        <f>G3</f>
-        <v>4</v>
-      </c>
-      <c r="J5" s="1">
-        <f>I3</f>
-        <v>6</v>
-      </c>
-      <c r="K5" s="1">
-        <f>K3</f>
-        <v>8</v>
-      </c>
-      <c r="L5" s="1">
-        <f>M3</f>
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C6" s="2">
         <f>L4</f>
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2">
         <f>J4</f>
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2">
         <f>H4</f>
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2">
         <f>F4</f>
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="G6" s="2">
         <f>D4</f>
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1">
         <f>E4</f>
-        <v>90</v>
+        <v>2</v>
       </c>
       <c r="I6" s="1">
         <f>G4</f>
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="J6" s="1">
         <f>I4</f>
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="K6" s="1">
         <f>K4</f>
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="L6" s="1">
         <f>M4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C7" s="2">
+        <f>L5</f>
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="G7">
-        <f>SUM(C6:G6)</f>
-        <v>409</v>
-      </c>
-      <c r="H7">
-        <f>SUM(H6:L6)</f>
-        <v>410</v>
+      <c r="D7" s="2">
+        <f>J5</f>
+        <v>75</v>
+      </c>
+      <c r="E7" s="2">
+        <f>H5</f>
+        <v>79</v>
+      </c>
+      <c r="F7" s="2">
+        <f>F5</f>
+        <v>89</v>
+      </c>
+      <c r="G7" s="2">
+        <f>D5</f>
+        <v>95</v>
+      </c>
+      <c r="H7" s="1">
+        <f>E5</f>
+        <v>90</v>
+      </c>
+      <c r="I7" s="1">
+        <f>G5</f>
+        <v>90</v>
+      </c>
+      <c r="J7" s="1">
+        <f>I5</f>
+        <v>84</v>
+      </c>
+      <c r="K7" s="1">
+        <f>K5</f>
+        <v>74</v>
+      </c>
+      <c r="L7" s="1">
+        <f>M5</f>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="I8">
-        <f xml:space="preserve"> G7-H7</f>
+      <c r="G8">
+        <f>SUM(C7:G7)</f>
+        <v>411</v>
+      </c>
+      <c r="H8">
+        <f>SUM(H7:L7)</f>
+        <v>408</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <f xml:space="preserve"> G8-H8</f>
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <f>F7-I7</f>
         <v>-1</v>
       </c>
-      <c r="J8">
-        <f>F6-I6</f>
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <f>I8-2*J8</f>
-        <v>-3</v>
-      </c>
-      <c r="L8">
-        <f>ABS(K8)</f>
-        <v>3</v>
-      </c>
-      <c r="M8">
-        <f>MIN(L8:L11)</f>
-        <v>3</v>
-      </c>
-      <c r="N8">
-        <f>MIN(M8,M13,M17,M20)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>-1</v>
-      </c>
-      <c r="D9">
-        <v>20</v>
-      </c>
-      <c r="E9">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <f>E6-J6</f>
-        <v>-5</v>
-      </c>
       <c r="K9">
-        <f>K8-2*J9</f>
-        <v>7</v>
+        <f>I9-2*J9</f>
+        <v>5</v>
       </c>
       <c r="L9">
         <f>ABS(K9)</f>
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <f>MIN(L9:L12)</f>
+        <v>5</v>
+      </c>
+      <c r="N9">
+        <f>MIN(M9,M14,M18,M21)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -805,27 +896,27 @@
         <v>20</v>
       </c>
       <c r="E10">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
         <v>2</v>
       </c>
       <c r="J10">
-        <f>D6-K6</f>
-        <v>1</v>
+        <f>E7-J7</f>
+        <v>-5</v>
       </c>
       <c r="K10">
         <f>K9-2*J10</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="L10">
         <f>ABS(K10)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -837,24 +928,24 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J11">
-        <f>C6-L6</f>
-        <v>-3</v>
+        <f>D7-K7</f>
+        <v>1</v>
       </c>
       <c r="K11">
         <f>K10-2*J11</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L11">
         <f>ABS(K11)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -863,15 +954,27 @@
         <v>20</v>
       </c>
       <c r="E12">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <f>C7-L7</f>
+        <v>3</v>
+      </c>
+      <c r="K12">
+        <f>K11-2*J12</f>
+        <v>7</v>
+      </c>
+      <c r="L12">
+        <f>ABS(K12)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -880,35 +983,15 @@
         <v>20</v>
       </c>
       <c r="E13">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13">
-        <f xml:space="preserve"> G7-H7</f>
-        <v>-1</v>
-      </c>
-      <c r="J13">
-        <f>E6-J6</f>
-        <v>-5</v>
-      </c>
-      <c r="K13">
-        <f>I13-2*J13</f>
-        <v>9</v>
-      </c>
-      <c r="L13">
-        <f>ABS(K13)</f>
-        <v>9</v>
-      </c>
-      <c r="M13">
-        <f>MIN(L13:L15)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -917,27 +1000,35 @@
         <v>20</v>
       </c>
       <c r="E14">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <f xml:space="preserve"> G8-H8</f>
+        <v>3</v>
       </c>
       <c r="J14">
-        <f>D6-K6</f>
-        <v>1</v>
+        <f>E7-J7</f>
+        <v>-5</v>
       </c>
       <c r="K14">
-        <f>K13-2*J14</f>
-        <v>7</v>
+        <f>I14-2*J14</f>
+        <v>13</v>
       </c>
       <c r="L14">
         <f>ABS(K14)</f>
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="M14">
+        <f>MIN(L14:L16)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -946,44 +1037,56 @@
         <v>20</v>
       </c>
       <c r="E15">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J15">
-        <f>C6-L6</f>
-        <v>-3</v>
+        <f>D7-K7</f>
+        <v>1</v>
       </c>
       <c r="K15">
         <f>K14-2*J15</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L15">
         <f>ABS(K15)</f>
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>-1</v>
       </c>
       <c r="D16">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E16">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <f>C7-L7</f>
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <f>K15-2*J16</f>
+        <v>5</v>
+      </c>
+      <c r="L16">
+        <f>ABS(K16)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -992,35 +1095,15 @@
         <v>40</v>
       </c>
       <c r="E17">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
-        <v>5</v>
-      </c>
-      <c r="I17">
-        <f xml:space="preserve"> G7-H7</f>
-        <v>-1</v>
-      </c>
-      <c r="J17">
-        <f>D6-K6</f>
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <f>I17-2*J17</f>
-        <v>-3</v>
-      </c>
-      <c r="L17">
-        <f>ABS(K17)</f>
-        <v>3</v>
-      </c>
-      <c r="M17">
-        <f>MIN(L17:L18)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -1029,27 +1112,35 @@
         <v>40</v>
       </c>
       <c r="E18">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <f xml:space="preserve"> G8-H8</f>
         <v>3</v>
       </c>
       <c r="J18">
-        <f>C6-L6</f>
-        <v>-3</v>
+        <f>D7-K7</f>
+        <v>1</v>
       </c>
       <c r="K18">
-        <f>K17-2*J18</f>
-        <v>3</v>
+        <f>I18-2*J18</f>
+        <v>1</v>
       </c>
       <c r="L18">
         <f>ABS(K18)</f>
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <f>MIN(L18:L19)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -1058,15 +1149,27 @@
         <v>40</v>
       </c>
       <c r="E19">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <f>C7-L7</f>
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <f>K18-2*J19</f>
+        <v>-5</v>
+      </c>
+      <c r="L19">
+        <f>ABS(K19)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -1075,35 +1178,15 @@
         <v>40</v>
       </c>
       <c r="E20">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>3</v>
-      </c>
-      <c r="I20">
-        <f xml:space="preserve"> G7-H7</f>
-        <v>-1</v>
-      </c>
-      <c r="J20">
-        <f>C6-L6</f>
-        <v>-3</v>
-      </c>
-      <c r="K20">
-        <f>I20-2*J20</f>
-        <v>5</v>
-      </c>
-      <c r="L20">
-        <f>ABS(K20)</f>
-        <v>5</v>
-      </c>
-      <c r="M20">
-        <f>MIN(L20)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -1112,15 +1195,35 @@
         <v>40</v>
       </c>
       <c r="E21">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F21" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="I21">
+        <f xml:space="preserve"> G8-H8</f>
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <f>C7-L7</f>
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <f>I21-2*J21</f>
+        <v>-3</v>
+      </c>
+      <c r="L21">
+        <f>ABS(K21)</f>
+        <v>3</v>
+      </c>
+      <c r="M21">
+        <f>MIN(L21)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -1129,38 +1232,15 @@
         <v>40</v>
       </c>
       <c r="E22">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F22" t="s">
         <v>4</v>
       </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3">
-        <f>G6</f>
-        <v>95</v>
-      </c>
-      <c r="K22" s="3">
-        <f>F6</f>
-        <v>90</v>
-      </c>
-      <c r="L22" s="3">
-        <f>E6</f>
-        <v>79</v>
-      </c>
-      <c r="M22" s="3">
-        <f>D6</f>
-        <v>75</v>
-      </c>
-      <c r="N22" s="3">
-        <f>C6</f>
-        <v>70</v>
-      </c>
-      <c r="O22" s="5"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -1169,123 +1249,118 @@
         <v>40</v>
       </c>
       <c r="E23">
+        <v>75</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3">
+        <f>G7</f>
+        <v>95</v>
+      </c>
+      <c r="K23" s="3">
+        <f>F7</f>
+        <v>89</v>
+      </c>
+      <c r="L23" s="3">
+        <f>E7</f>
         <v>79</v>
       </c>
-      <c r="F23" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6">
-        <v>1</v>
-      </c>
-      <c r="K23" s="6">
-        <v>3</v>
-      </c>
-      <c r="L23" s="6">
-        <v>5</v>
-      </c>
-      <c r="M23" s="6">
-        <v>7</v>
-      </c>
-      <c r="N23" s="6">
-        <v>9</v>
+      <c r="M23" s="3">
+        <f>D7</f>
+        <v>75</v>
+      </c>
+      <c r="N23" s="3">
+        <f>C7</f>
+        <v>73</v>
       </c>
       <c r="O23" s="5"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C24">
         <v>-1</v>
       </c>
       <c r="D24">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E24">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F24" t="s">
         <v>2</v>
       </c>
-      <c r="H24" s="3">
-        <f>H6</f>
-        <v>90</v>
-      </c>
-      <c r="I24" s="6">
-        <v>2</v>
-      </c>
+      <c r="H24" s="3"/>
+      <c r="I24" s="6"/>
       <c r="J24" s="6">
-        <f>MIN(K24:N24)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K24" s="6">
-        <f>MIN(ABS(K25),ABS(L25),ABS(M25),ABS(N25))</f>
         <v>3</v>
       </c>
       <c r="L24" s="6">
-        <f>MIN(ABS(L26),ABS(M26),ABS(N26))</f>
+        <v>5</v>
+      </c>
+      <c r="M24" s="6">
         <v>7</v>
       </c>
-      <c r="M24" s="6">
-        <f>MIN(ABS(M27),ABS(N27))</f>
-        <v>3</v>
-      </c>
       <c r="N24" s="6">
-        <f>MIN(ABS(N28))</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="O24" s="5"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C25">
         <v>-1</v>
       </c>
       <c r="D25">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E25">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F25" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H25" s="3">
-        <f>I6</f>
-        <v>89</v>
+        <f>H7</f>
+        <v>90</v>
       </c>
       <c r="I25" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J25" s="6">
-        <f>G7-H7</f>
-        <v>-1</v>
-      </c>
-      <c r="K25" s="8">
-        <f>J25-(K22-H25)*2</f>
-        <v>-3</v>
-      </c>
-      <c r="L25" s="7">
-        <f>K25-2*(L22-H26)</f>
-        <v>7</v>
-      </c>
-      <c r="M25" s="7">
-        <f>L25-2*(M22-H27)</f>
-        <v>5</v>
-      </c>
-      <c r="N25" s="7">
-        <f>M25-2*(N22-H28)</f>
-        <v>11</v>
-      </c>
-      <c r="O25" s="4"/>
+        <f>MIN(K25:N25)</f>
+        <v>1</v>
+      </c>
+      <c r="K25" s="6">
+        <f>MIN(ABS(K26),ABS(L26),ABS(M26),ABS(N26))</f>
+        <v>5</v>
+      </c>
+      <c r="L25" s="6">
+        <f>MIN(ABS(L27),ABS(M27),ABS(N27))</f>
+        <v>5</v>
+      </c>
+      <c r="M25" s="6">
+        <f>MIN(ABS(M28),ABS(N28))</f>
+        <v>1</v>
+      </c>
+      <c r="N25" s="6">
+        <f>MIN(ABS(N29))</f>
+        <v>3</v>
+      </c>
+      <c r="O25" s="5"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -1294,42 +1369,43 @@
         <v>40</v>
       </c>
       <c r="E26">
+        <v>89</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="3">
+        <f>I7</f>
         <v>90</v>
       </c>
-      <c r="F26" t="s">
-        <v>2</v>
-      </c>
-      <c r="H26" s="3">
-        <f>J6</f>
-        <v>84</v>
-      </c>
       <c r="I26" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J26" s="6">
-        <v>0</v>
-      </c>
-      <c r="K26" s="6">
-        <f>G7-H7</f>
-        <v>-1</v>
-      </c>
-      <c r="L26" s="8">
-        <f>K26-2*(L22-H26)</f>
-        <v>9</v>
+        <f>G8-H8</f>
+        <v>3</v>
+      </c>
+      <c r="K26" s="8">
+        <f>J26-(K23-H26)*2</f>
+        <v>5</v>
+      </c>
+      <c r="L26" s="7">
+        <f>K26-2*(L23-H27)</f>
+        <v>15</v>
       </c>
       <c r="M26" s="7">
-        <f>L26-2*(M22-H27)</f>
+        <f>L26-2*(M23-H28)</f>
+        <v>13</v>
+      </c>
+      <c r="N26" s="7">
+        <f>M26-2*(N23-H29)</f>
         <v>7</v>
-      </c>
-      <c r="N26" s="7">
-        <f>M26-2*(N22-H28)</f>
-        <v>13</v>
       </c>
       <c r="O26" s="4"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B27">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -1341,38 +1417,39 @@
         <v>90</v>
       </c>
       <c r="F27" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="3">
+        <f>J7</f>
+        <v>84</v>
+      </c>
+      <c r="I27" s="6">
         <v>6</v>
-      </c>
-      <c r="H27" s="3">
-        <f>K6</f>
-        <v>74</v>
-      </c>
-      <c r="I27" s="6">
-        <v>8</v>
       </c>
       <c r="J27" s="6">
         <v>0</v>
       </c>
       <c r="K27" s="6">
-        <v>0</v>
-      </c>
-      <c r="L27" s="6">
-        <f>G7-H7</f>
-        <v>-1</v>
-      </c>
-      <c r="M27" s="8">
-        <f>L27-2*(M22-H27)</f>
-        <v>-3</v>
+        <f>G8-H8</f>
+        <v>3</v>
+      </c>
+      <c r="L27" s="8">
+        <f>K27-2*(L23-H27)</f>
+        <v>13</v>
+      </c>
+      <c r="M27" s="7">
+        <f>L27-2*(M23-H28)</f>
+        <v>11</v>
       </c>
       <c r="N27" s="7">
-        <f>M27-2*(N22-H28)</f>
-        <v>3</v>
+        <f>M27-2*(N23-H29)</f>
+        <v>5</v>
       </c>
       <c r="O27" s="4"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B28">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -1381,17 +1458,17 @@
         <v>40</v>
       </c>
       <c r="E28">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F28" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H28" s="3">
-        <f>L6</f>
-        <v>73</v>
+        <f>K7</f>
+        <v>74</v>
       </c>
       <c r="I28" s="6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J28" s="6">
         <v>0</v>
@@ -1400,94 +1477,123 @@
         <v>0</v>
       </c>
       <c r="L28" s="6">
+        <f>G8-H8</f>
+        <v>3</v>
+      </c>
+      <c r="M28" s="8">
+        <f>L28-2*(M23-H28)</f>
+        <v>1</v>
+      </c>
+      <c r="N28" s="7">
+        <f>M28-2*(N23-H29)</f>
+        <v>-5</v>
+      </c>
+      <c r="O28" s="4"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>-1</v>
+      </c>
+      <c r="D29">
+        <v>40</v>
+      </c>
+      <c r="E29">
+        <v>95</v>
+      </c>
+      <c r="F29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="3">
+        <f>L7</f>
+        <v>70</v>
+      </c>
+      <c r="I29" s="6">
+        <v>10</v>
+      </c>
+      <c r="J29" s="6">
         <v>0</v>
       </c>
-      <c r="M28" s="6">
-        <f>G7-H7</f>
-        <v>-1</v>
-      </c>
-      <c r="N28" s="8">
-        <f>M28-2*(N22-H28)</f>
-        <v>5</v>
-      </c>
-      <c r="O28" s="4"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I32" t="s">
-        <v>8</v>
-      </c>
-      <c r="K32" t="s">
-        <v>10</v>
-      </c>
-      <c r="M32" t="s">
-        <v>11</v>
-      </c>
-      <c r="O32" t="s">
-        <v>12</v>
-      </c>
+      <c r="K29" s="6">
+        <v>0</v>
+      </c>
+      <c r="L29" s="6">
+        <v>0</v>
+      </c>
+      <c r="M29" s="6">
+        <f>G8-H8</f>
+        <v>3</v>
+      </c>
+      <c r="N29" s="8">
+        <f>M29-2*(N23-H29)</f>
+        <v>-3</v>
+      </c>
+      <c r="O29" s="4"/>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.3">
       <c r="I33" t="s">
+        <v>8</v>
+      </c>
+      <c r="K33" t="s">
+        <v>10</v>
+      </c>
+      <c r="M33" t="s">
+        <v>11</v>
+      </c>
+      <c r="O33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="I34" t="s">
         <v>9</v>
       </c>
-      <c r="M33" t="s">
+      <c r="M34" t="s">
         <v>13</v>
       </c>
-      <c r="O33" t="s">
+      <c r="O34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="E35" t="s">
+    <row r="36" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="E36" s="9" t="s">
+    <row r="37" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="E37" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F37" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G37" s="9" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="D37" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G37" s="9">
-        <v>1</v>
-      </c>
-      <c r="J37" t="s">
-        <v>14</v>
-      </c>
-      <c r="K37" t="s">
-        <v>15</v>
-      </c>
-      <c r="L37" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G38" s="9">
         <v>1</v>
+      </c>
+      <c r="J38" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" t="s">
+        <v>15</v>
+      </c>
+      <c r="L38" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.3">
@@ -1495,7 +1601,7 @@
         <v>33</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>34</v>
@@ -1503,92 +1609,75 @@
       <c r="G39" s="9">
         <v>1</v>
       </c>
-      <c r="J39" t="s">
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="9">
+        <v>1</v>
+      </c>
+      <c r="J40" t="s">
         <v>17</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L40" t="s">
         <v>18</v>
       </c>
-      <c r="N39">
+      <c r="N40">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="G40">
-        <v>1</v>
-      </c>
-    </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="E41" s="9" t="s">
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="E42" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F42" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G42" s="9" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="D42" t="s">
-        <v>32</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G42" s="9">
-        <v>1</v>
-      </c>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3">
-        <v>100</v>
-      </c>
-      <c r="K42" s="3">
-        <v>40</v>
-      </c>
-      <c r="L42" s="3">
-        <v>28</v>
-      </c>
-      <c r="M42" s="3">
-        <v>19</v>
-      </c>
-      <c r="N42" s="3">
-        <v>0</v>
       </c>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G43" s="9">
         <v>1</v>
       </c>
       <c r="H43" s="3"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6">
-        <v>1</v>
-      </c>
-      <c r="K43" s="6">
-        <v>3</v>
-      </c>
-      <c r="L43" s="6">
-        <v>5</v>
-      </c>
-      <c r="M43" s="6">
-        <v>7</v>
-      </c>
-      <c r="N43" s="6">
-        <v>9</v>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3">
+        <v>100</v>
+      </c>
+      <c r="K43" s="3">
+        <v>40</v>
+      </c>
+      <c r="L43" s="3">
+        <v>28</v>
+      </c>
+      <c r="M43" s="3">
+        <v>19</v>
+      </c>
+      <c r="N43" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.3">
@@ -1596,109 +1685,113 @@
         <v>33</v>
       </c>
       <c r="E44" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G44" s="9">
+        <v>1</v>
+      </c>
+      <c r="H44" s="3"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6">
+        <v>1</v>
+      </c>
+      <c r="K44" s="6">
+        <v>3</v>
+      </c>
+      <c r="L44" s="6">
+        <v>5</v>
+      </c>
+      <c r="M44" s="6">
+        <v>7</v>
+      </c>
+      <c r="N44" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F44" s="9" t="s">
+      <c r="F45" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G44" s="9">
-        <v>1</v>
-      </c>
-      <c r="H44" s="3">
+      <c r="G45" s="9">
+        <v>1</v>
+      </c>
+      <c r="H45" s="3">
         <v>65</v>
       </c>
-      <c r="I44" s="6">
-        <v>2</v>
-      </c>
-      <c r="J44" s="6">
+      <c r="I45" s="6">
+        <v>2</v>
+      </c>
+      <c r="J45" s="6">
         <v>0</v>
       </c>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
-    </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="H45" s="3">
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+    </row>
+    <row r="46" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="H46" s="3">
         <v>32</v>
       </c>
-      <c r="I45" s="6">
+      <c r="I46" s="6">
         <v>4</v>
       </c>
-      <c r="J45" s="6">
+      <c r="J46" s="6">
         <v>70</v>
       </c>
-      <c r="K45" s="8">
+      <c r="K46" s="8">
         <v>54</v>
       </c>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
-    </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C46">
-        <v>10</v>
-      </c>
-      <c r="D46">
-        <v>10</v>
-      </c>
-      <c r="E46">
-        <v>8</v>
-      </c>
-      <c r="H46" s="3">
-        <v>20</v>
-      </c>
-      <c r="I46" s="6">
-        <v>6</v>
-      </c>
-      <c r="J46" s="6">
-        <v>0</v>
-      </c>
-      <c r="K46" s="6">
-        <v>70</v>
-      </c>
-      <c r="L46" s="8">
-        <v>54</v>
-      </c>
+      <c r="L46" s="7"/>
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
     </row>
     <row r="47" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>10</v>
+      </c>
       <c r="E47">
+        <v>8</v>
+      </c>
+      <c r="H47" s="3">
+        <v>20</v>
+      </c>
+      <c r="I47" s="6">
         <v>6</v>
-      </c>
-      <c r="H47" s="3">
-        <v>0</v>
-      </c>
-      <c r="I47" s="6">
-        <v>8</v>
       </c>
       <c r="J47" s="6">
         <v>0</v>
       </c>
       <c r="K47" s="6">
-        <v>0</v>
-      </c>
-      <c r="L47" s="6">
         <v>70</v>
       </c>
-      <c r="M47" s="8">
-        <v>32</v>
-      </c>
+      <c r="L47" s="8">
+        <v>54</v>
+      </c>
+      <c r="M47" s="7"/>
       <c r="N47" s="7"/>
     </row>
     <row r="48" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C48" t="s">
-        <v>35</v>
-      </c>
       <c r="E48">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H48" s="3">
         <v>0</v>
       </c>
       <c r="I48" s="6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J48" s="6">
         <v>0</v>
@@ -1707,199 +1800,541 @@
         <v>0</v>
       </c>
       <c r="L48" s="6">
+        <v>70</v>
+      </c>
+      <c r="M48" s="8">
+        <v>32</v>
+      </c>
+      <c r="N48" s="7"/>
+    </row>
+    <row r="49" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>35</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="H49" s="3">
         <v>0</v>
       </c>
-      <c r="M48" s="6">
+      <c r="I49" s="6">
+        <v>10</v>
+      </c>
+      <c r="J49" s="6">
+        <v>0</v>
+      </c>
+      <c r="K49" s="6">
+        <v>0</v>
+      </c>
+      <c r="L49" s="6">
+        <v>0</v>
+      </c>
+      <c r="M49" s="6">
         <v>70</v>
       </c>
-      <c r="N48" s="8">
+      <c r="N49" s="8">
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="E49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:15" x14ac:dyDescent="0.3">
       <c r="E50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="E51">
         <v>0</v>
       </c>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10">
-        <v>1</v>
-      </c>
-      <c r="L50">
-        <v>2</v>
-      </c>
-      <c r="M50">
-        <v>3</v>
-      </c>
-      <c r="N50">
+      <c r="J51" s="10"/>
+      <c r="K51" s="10">
+        <v>1</v>
+      </c>
+      <c r="L51">
+        <v>2</v>
+      </c>
+      <c r="M51">
+        <v>3</v>
+      </c>
+      <c r="N51">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="H51" t="s">
+    <row r="52" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="H52" t="s">
         <v>14</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I52" t="s">
         <v>22</v>
       </c>
-      <c r="J51" s="6"/>
-      <c r="K51" s="11">
+      <c r="J52" s="6"/>
+      <c r="K52" s="11">
         <v>-3</v>
       </c>
-      <c r="L51" s="11">
+      <c r="L52" s="11">
         <v>9</v>
       </c>
-      <c r="M51" s="11">
+      <c r="M52" s="11">
         <v>-3</v>
       </c>
-      <c r="N51" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="I52" t="s">
+      <c r="N52" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="I53" t="s">
         <v>24</v>
       </c>
-      <c r="J52">
-        <v>1</v>
-      </c>
-      <c r="K52" s="9"/>
-      <c r="L52" s="9"/>
-      <c r="M52" s="9"/>
-      <c r="N52" s="9"/>
-      <c r="O52" s="9"/>
-    </row>
-    <row r="53" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="H53" t="s">
-        <v>23</v>
-      </c>
-      <c r="I53" t="s">
-        <v>21</v>
-      </c>
-      <c r="J53" s="9">
-        <v>2</v>
-      </c>
-      <c r="K53" s="9">
-        <v>4</v>
-      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53" s="9"/>
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
     </row>
-    <row r="54" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="H54" t="s">
+        <v>23</v>
+      </c>
       <c r="I54" t="s">
+        <v>21</v>
+      </c>
+      <c r="J54" s="9">
+        <v>2</v>
+      </c>
+      <c r="K54" s="9">
+        <v>4</v>
+      </c>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
+      <c r="O54" s="9"/>
+    </row>
+    <row r="55" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="I55" t="s">
         <v>19</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J55" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="I55" t="s">
+    <row r="56" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="I56" t="s">
         <v>14</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J56" t="s">
         <v>39</v>
       </c>
-      <c r="K55" t="s">
+      <c r="K56" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="I56" s="9">
+    <row r="57" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="I57" s="9">
         <v>13</v>
       </c>
-      <c r="J56">
-        <v>3</v>
-      </c>
-      <c r="K56">
+      <c r="J57">
+        <v>3</v>
+      </c>
+      <c r="K57">
         <v>-3</v>
       </c>
     </row>
-    <row r="57" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="I57" s="9">
-        <v>5</v>
-      </c>
-      <c r="J57">
+    <row r="58" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="I58" s="9">
+        <v>5</v>
+      </c>
+      <c r="J58">
         <v>15</v>
       </c>
-      <c r="K57">
+      <c r="K58">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="I58" s="9">
+    <row r="59" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="I59" s="9">
         <v>13</v>
       </c>
-      <c r="J58">
-        <v>3</v>
-      </c>
-      <c r="K58">
+      <c r="J59">
+        <v>3</v>
+      </c>
+      <c r="K59">
         <v>-3</v>
       </c>
     </row>
-    <row r="59" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="I59" s="9">
+    <row r="60" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="I60" s="9">
         <v>9</v>
       </c>
-      <c r="J59">
+      <c r="J60">
         <v>-1</v>
       </c>
-      <c r="K59">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="H61" s="9">
+      <c r="K60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="H62" s="9">
         <v>15</v>
       </c>
-      <c r="I61" s="9">
-        <v>5</v>
-      </c>
-      <c r="J61" s="9">
-        <v>1</v>
-      </c>
-      <c r="K61" s="9">
-        <v>1</v>
-      </c>
-      <c r="L61" s="9"/>
-      <c r="M61" s="9"/>
-    </row>
-    <row r="63" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="E63" t="s">
+      <c r="I62" s="9">
+        <v>5</v>
+      </c>
+      <c r="J62" s="9">
+        <v>1</v>
+      </c>
+      <c r="K62" s="9">
+        <v>1</v>
+      </c>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+    </row>
+    <row r="64" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="E64" t="s">
         <v>36</v>
       </c>
-      <c r="L63">
-        <v>2</v>
-      </c>
-      <c r="M63">
+      <c r="L64">
+        <v>2</v>
+      </c>
+      <c r="M64">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="E64" s="12" t="s">
+    <row r="65" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E65" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+    </row>
+    <row r="83" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83">
+        <v>95</v>
+      </c>
+      <c r="D83">
+        <v>90</v>
+      </c>
+      <c r="E83">
+        <v>90</v>
+      </c>
+      <c r="F83">
+        <v>89</v>
+      </c>
+      <c r="G83">
+        <v>84</v>
+      </c>
+      <c r="H83">
+        <v>79</v>
+      </c>
+      <c r="I83">
+        <v>75</v>
+      </c>
+      <c r="J83">
+        <v>74</v>
+      </c>
+      <c r="K83">
+        <v>73</v>
+      </c>
+      <c r="L83">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="87" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>39</v>
+      </c>
+      <c r="C87" s="9">
+        <v>95</v>
+      </c>
+      <c r="D87" s="9">
+        <v>89</v>
+      </c>
+      <c r="E87" s="9">
+        <v>79</v>
+      </c>
+      <c r="F87" s="9">
+        <v>75</v>
+      </c>
+      <c r="G87" s="9">
+        <v>73</v>
+      </c>
+      <c r="H87" s="9">
+        <f>SUM(C87:G87)</f>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="88" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="J88">
+        <f>ABS(H87-H89)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C89" s="9">
+        <v>90</v>
+      </c>
+      <c r="D89" s="9">
+        <v>90</v>
+      </c>
+      <c r="E89" s="9">
+        <v>84</v>
+      </c>
+      <c r="F89" s="9">
+        <v>74</v>
+      </c>
+      <c r="G89" s="13">
+        <v>70</v>
+      </c>
+      <c r="H89" s="9">
+        <f>SUM(C89:G89)</f>
+        <v>408</v>
+      </c>
+    </row>
+    <row r="90" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C90" t="s">
+        <v>42</v>
+      </c>
+      <c r="M90">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>2</v>
+      </c>
+      <c r="E92">
+        <v>3</v>
+      </c>
+      <c r="F92">
+        <v>4</v>
+      </c>
+      <c r="G92">
+        <v>5</v>
+      </c>
+      <c r="H92">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" t="s">
+        <v>45</v>
+      </c>
+      <c r="D93" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="94" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C94" t="s">
+        <v>47</v>
+      </c>
+      <c r="D94" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C95" t="s">
+        <v>49</v>
+      </c>
+      <c r="D95" t="s">
+        <v>50</v>
+      </c>
+      <c r="M95">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="96" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C96" t="s">
+        <v>43</v>
+      </c>
+      <c r="D96" t="s">
+        <v>44</v>
+      </c>
+      <c r="E96" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C97" t="s">
+        <v>56</v>
+      </c>
+      <c r="D97" t="s">
+        <v>52</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97" t="s">
+        <v>53</v>
+      </c>
+      <c r="H97" t="s">
+        <v>54</v>
+      </c>
+      <c r="I97" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>2</v>
+      </c>
+      <c r="E100">
+        <v>3</v>
+      </c>
+      <c r="F100">
+        <v>4</v>
+      </c>
+      <c r="G100">
+        <v>5</v>
+      </c>
+      <c r="H100">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>14</v>
+      </c>
+      <c r="C101" s="14">
+        <v>2</v>
+      </c>
+      <c r="D101" s="14">
+        <v>1</v>
+      </c>
+      <c r="E101" s="14">
+        <v>7</v>
+      </c>
+      <c r="F101" s="15">
+        <v>9</v>
+      </c>
+      <c r="G101" s="15">
+        <v>6</v>
+      </c>
+      <c r="H101" s="15">
+        <v>5</v>
+      </c>
+      <c r="I101">
+        <f>SUM(C101:H101)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>57</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>2</v>
+      </c>
+      <c r="F102">
+        <v>3</v>
+      </c>
+      <c r="G102">
+        <v>4</v>
+      </c>
+      <c r="H102">
+        <v>5</v>
+      </c>
+      <c r="I102">
+        <v>6</v>
+      </c>
+      <c r="J102">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>59</v>
+      </c>
+      <c r="B103" t="s">
+        <v>58</v>
+      </c>
+      <c r="C103" s="9">
+        <v>0</v>
+      </c>
+      <c r="D103" s="9">
+        <v>2</v>
+      </c>
+      <c r="E103" s="9">
+        <v>1</v>
+      </c>
+      <c r="F103" s="9">
+        <v>2</v>
+      </c>
+      <c r="G103" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H103" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I103" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J103" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="K103" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L103" s="9"/>
+      <c r="M103" s="9"/>
+      <c r="N103" s="9"/>
+      <c r="O103" s="9"/>
+      <c r="P103" s="9"/>
+      <c r="Q103" s="9"/>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B107">
+        <v>3</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <v>2</v>
+      </c>
+      <c r="F107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="E109">
+        <f>B107-C107</f>
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="B9:F28">
     <sortCondition ref="E32"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="E64:I64"/>
+    <mergeCell ref="E65:I65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>